<commit_message>
Update to the Package dimension mapping after speaking with Haug. This will help narrow down the sources for the mapping of the Features.
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Package.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Package.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359E2608-96B4-448E-AC9E-C42D998FC98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0335C7-73FF-44B1-B1BF-623E67D60754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Package" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="35">
   <si>
     <t>Database</t>
   </si>
@@ -122,18 +122,6 @@
   </si>
   <si>
     <t>FS_Retail_Price</t>
-  </si>
-  <si>
-    <t>Source-2</t>
-  </si>
-  <si>
-    <t>Source-3</t>
-  </si>
-  <si>
-    <t>FEA_ID</t>
-  </si>
-  <si>
-    <t>FEA_Type</t>
   </si>
   <si>
     <t>FEA_Value</t>
@@ -160,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,20 +167,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="45"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="41"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -239,24 +215,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -269,30 +232,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="G2" sqref="G1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -623,37 +572,21 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-    </row>
-    <row r="2" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -672,26 +605,8 @@
       <c r="F2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -701,19 +616,13 @@
       <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -732,14 +641,8 @@
       <c r="F4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-    </row>
-    <row r="5" spans="1:12" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -758,14 +661,8 @@
       <c r="F5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-    </row>
-    <row r="6" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -782,28 +679,10 @@
         <v>30</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -820,28 +699,10 @@
         <v>30</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -858,28 +719,10 @@
         <v>30</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="6" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -896,28 +739,10 @@
         <v>30</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -934,28 +759,10 @@
         <v>30</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
@@ -972,28 +779,10 @@
         <v>30</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1010,28 +799,10 @@
         <v>30</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1048,28 +819,10 @@
         <v>30</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J13" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K13" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1086,28 +839,10 @@
         <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>5</v>
       </c>
@@ -1124,28 +859,10 @@
         <v>30</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L15" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
@@ -1162,28 +879,10 @@
         <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>5</v>
       </c>
@@ -1200,28 +899,10 @@
         <v>30</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -1238,28 +919,10 @@
         <v>30</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
@@ -1276,28 +939,10 @@
         <v>30</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H19" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J19" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K19" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -1314,28 +959,10 @@
         <v>30</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>5</v>
       </c>
@@ -1352,28 +979,10 @@
         <v>30</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K21" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
@@ -1390,28 +999,10 @@
         <v>30</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
@@ -1428,34 +1019,14 @@
         <v>30</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="J23" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="K23" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L23" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>